<commit_message>
Added alcholic class specials.
</commit_message>
<xml_diff>
--- a/resources/data-imports/All (Affixes).xlsx
+++ b/resources/data-imports/All (Affixes).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="947">
   <si>
     <t>id</t>
   </si>
@@ -638,7 +638,7 @@
     <t>Faithless Hate</t>
   </si>
   <si>
-    <t>There is nothing worse then the hatefilled vengance of the faithless.</t>
+    <t>There is nothing worse then the hate filled vengeance of the faithless.</t>
   </si>
   <si>
     <t>Blessed Treasures</t>
@@ -662,7 +662,7 @@
     <t>Dodge</t>
   </si>
   <si>
-    <t>Devils Deliverence</t>
+    <t>Devils Deliverance</t>
   </si>
   <si>
     <t>Let the devil deliver this aim child!</t>
@@ -683,10 +683,10 @@
     <t>The Plague</t>
   </si>
   <si>
-    <t>Medatative Hope</t>
-  </si>
-  <si>
-    <t>As you meditate, get a sense of feeling hope course through your viens</t>
+    <t>Meditative Hope</t>
+  </si>
+  <si>
+    <t>As you meditate, get a sense of feeling hope course through your veins</t>
   </si>
   <si>
     <t>Mages Devilish Deeds</t>
@@ -989,7 +989,7 @@
     <t>Sickness in the Soul</t>
   </si>
   <si>
-    <t>Debilitating sickness takes over the enemy. This is a Stat reduction prefix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
+    <t>Debilitating sickness takes over the enemy. This is a Stat reduction suffix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
   </si>
   <si>
     <t>Faithless Slaughter</t>
@@ -1037,7 +1037,10 @@
     <t>Thousand Thoughts</t>
   </si>
   <si>
-    <t>Trained Bowmen's Blood</t>
+    <t>The enemy loses their focus. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
+    <t>Trained Bowman's Blood</t>
   </si>
   <si>
     <t>Apparently, bleeding out a trained bowmen and pouring his blood over the bow increases your ability to hit anything. How amazing.</t>
@@ -1112,7 +1115,7 @@
     <t>Kings Quest</t>
   </si>
   <si>
-    <t>The quest that’s imbued with in this enchantment is said to be a legendary unlockable quest that gives you unlimited power.</t>
+    <t>The quest that’s imbued with in this enchantment is said to be a legendary unlock-able quest that gives you unlimited power.</t>
   </si>
   <si>
     <t>The Creators Blessing</t>
@@ -1337,7 +1340,7 @@
     <t>Let time be on your side, child.</t>
   </si>
   <si>
-    <t>Lifes Dance</t>
+    <t>Life's Dance</t>
   </si>
   <si>
     <t>Dance to the song of life child.</t>
@@ -1400,7 +1403,7 @@
     <t>Angelic Light</t>
   </si>
   <si>
-    <t>The enemy is overtaken by the light of the Angels. They become weaker. This is a Stat reduction prefix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
+    <t>The enemy is overtaken by the light of the Angels. They become weaker. This is a Stat reduction suffix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
   </si>
   <si>
     <t>Arch Mages Wrath</t>
@@ -1415,7 +1418,7 @@
     <t>Have faith in the Lord of Light and you shall prevail</t>
   </si>
   <si>
-    <t>Devlish Strength</t>
+    <t>Devilish Strength</t>
   </si>
   <si>
     <t>What pact did you make to get the strength you have now child?</t>
@@ -1433,7 +1436,7 @@
     <t>Move quickly with pace of a cat. Claws as sharp as a cat's to slit the enemies throat.</t>
   </si>
   <si>
-    <t>Dextrous Infatuation</t>
+    <t>Dexterous Infatuation</t>
   </si>
   <si>
     <t>Infatuated with being able to hit things is a good thing child.</t>
@@ -1469,7 +1472,7 @@
     <t>Three rings entwined in a knot make up the magical glowing symbol upon your gear.</t>
   </si>
   <si>
-    <t>Cry of Maddness</t>
+    <t>Cry of Madness</t>
   </si>
   <si>
     <t>The enemy cries out in madness. This is a Entrancing enchantment that can be resisted if you do not have the right quest item. This item has a % chance to "entrance" the enemy, making them unable to block or dodge. This takes effect before all other enchantments and your attacks.</t>
@@ -1682,7 +1685,7 @@
     <t>Harbinger of Blood</t>
   </si>
   <si>
-    <t>When you enter the room, people just fall to the ground bleedig to death. The blood lust is so strong.</t>
+    <t>When you enter the room, people just fall to the ground bleeding to death. The blood lust is so strong.</t>
   </si>
   <si>
     <t>Insanity</t>
@@ -1718,6 +1721,9 @@
     <t>Dumbfounded</t>
   </si>
   <si>
+    <t>Drain the enemies intelligence. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
     <t>Fairy Trix</t>
   </si>
   <si>
@@ -1727,19 +1733,22 @@
     <t>Loss of Time</t>
   </si>
   <si>
+    <t>The enemies agility falls. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
     <t>Godly Love</t>
   </si>
   <si>
     <t>Let the love of God into your heart, let him fill you with hopes and dreams.</t>
   </si>
   <si>
-    <t>Childs Wonder</t>
+    <t>Child's Wonder</t>
   </si>
   <si>
     <t>Grimoire Enchantments</t>
   </si>
   <si>
-    <t>Many witches places magical spells upon their grimoires, these enchantments will raidate through out your gear.</t>
+    <t>Many witches places magical spells upon their grimoires, these enchantments will radiate through out your gear.</t>
   </si>
   <si>
     <t>Devils Ambition</t>
@@ -1787,7 +1796,7 @@
     <t>Rage of The hammer</t>
   </si>
   <si>
-    <t>Let the rage of your hammer break through the defences of the enemy.</t>
+    <t>Let the rage of your hammer break through the defenses of the enemy.</t>
   </si>
   <si>
     <t>Wizards Curse</t>
@@ -1820,7 +1829,7 @@
     <t>Embers of Smithy</t>
   </si>
   <si>
-    <t>Let the fires of the smithies workshop flow through your viens.</t>
+    <t>Let the fires of the smithies workshop flow through your veins</t>
   </si>
   <si>
     <t>Deep Cut</t>
@@ -1877,7 +1886,7 @@
     <t>Deaths Enchanter</t>
   </si>
   <si>
-    <t>Allow death to be your enchanter, more specifically his second in command who is also an enchanter. Let his magics flow through you when ehcnating.</t>
+    <t>Allow death to be your enchanter, more specifically his second in command who is also an enchanter. Let his magics flow through you when enchanting.</t>
   </si>
   <si>
     <t>Earth Tuned</t>
@@ -1907,7 +1916,7 @@
     <t>Wizards Mutterings</t>
   </si>
   <si>
-    <t>The mutterings of a wizard are said to flow through this enchantment. The muttering sof the wise and the faithful to the true art of magic.</t>
+    <t>The mutterings of a wizard are said to flow through this enchantment. The mutterings of the wise and the faithful to the true art of magic.</t>
   </si>
   <si>
     <t>Faithless Raging Temptation</t>
@@ -1949,6 +1958,9 @@
     <t>Fear</t>
   </si>
   <si>
+    <t>Lower the strength from your enemy. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
     <t>Time Battler's Blood</t>
   </si>
   <si>
@@ -1958,10 +1970,16 @@
     <t>Bleeding Gash</t>
   </si>
   <si>
-    <t>Ilussionary Work</t>
-  </si>
-  <si>
-    <t>Demonic Acuracy</t>
+    <t>Make the enemies durability fall. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
+    <t>Illusionary Work</t>
+  </si>
+  <si>
+    <t>Reduce the enemies dexterity. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
+    <t>Demonic Accuracy</t>
   </si>
   <si>
     <t>Praying and working with demons can get you the ability to aim better, but at what cost?</t>
@@ -2075,7 +2093,7 @@
     <t>Thieves Blood</t>
   </si>
   <si>
-    <t>Using the blood of theieves before you, this enchantment was woven out of their accomplishments and failures.</t>
+    <t>Using the blood of thieves before you, this enchantment was woven out of their accomplishments and failures.</t>
   </si>
   <si>
     <t>Demonic Soldier</t>
@@ -2123,7 +2141,7 @@
     <t>Queen Of Enchants</t>
   </si>
   <si>
-    <t>The queen of enchanting has created her own enchantment to help those who want to learnt he craft become better, almost instantly then those who had to work long and hard.</t>
+    <t>The queen of enchanting has created her own enchantment to help those who want to learn the craft become better, almost instantly then those who had to work long and hard.</t>
   </si>
   <si>
     <t>Demons Claws</t>
@@ -2147,7 +2165,7 @@
     <t>Schizophrenic Attack</t>
   </si>
   <si>
-    <t>The enemy has a terrible schizophrenic attack.This is a Entrancing enchantment that can be resisted if you do not have the right quest item. This item has a % chance to "entrance" the enemy, making them unable to block or dodge. This takes effect before all other enchantments and your attacks.</t>
+    <t>The enemy has a terrible schizophrenic attack. This is a Entrancing enchantment that can be resisted if you do not have the right quest item. This item has a % chance to "entrance" the enemy, making them unable to block or dodge. This takes effect before all other enchantments and your attacks.</t>
   </si>
   <si>
     <t>Nature's Anger</t>
@@ -2240,7 +2258,7 @@
     <t>Brimstone</t>
   </si>
   <si>
-    <t>The skys open, fire rains down with large chunks of sulfur smelling brimstone. The enemy will surley die! This type of affix can do damage and may or may not stack with the more you have equipped. Check the details below. Damaging affixes can be resisted by enemies unless otherwise stated.</t>
+    <t>The sky's open, fire rains down with large chunks of sulfur smelling brimstone. The enemy will surely die! This type of affix can do damage and may or may not stack with the more you have equipped. Check the details below. Damaging affixes can be resisted by enemies unless otherwise stated.</t>
   </si>
   <si>
     <t>Godly Aspirations</t>
@@ -2309,6 +2327,9 @@
     <t>Godless Heathen</t>
   </si>
   <si>
+    <t>The enemies chr will fall. This is a Stat reduction prefix. These do stack and will be added to any prefix in which all enemy stats are reduced. This enchantment can be resisted, unless you have the appropriate quest item.</t>
+  </si>
+  <si>
     <t>Bleeding Brain</t>
   </si>
   <si>
@@ -2336,7 +2357,7 @@
     <t>Puff of Smoke</t>
   </si>
   <si>
-    <t>Disapear through a puff of smoke</t>
+    <t>Disappear through a puff of smoke</t>
   </si>
   <si>
     <t>Shadow Nature</t>
@@ -2363,6 +2384,9 @@
     <t>Shadow Fury</t>
   </si>
   <si>
+    <t>The sky s open, fire rains down with large chunks of sulfur smelling brimstone. The enemy will surely die! This type of affix can do damage and may or may not stack with the more you have equipped. Check the details below. Damaging affixes can be resisted by enemies unless otherwise stated.</t>
+  </si>
+  <si>
     <t>Double the Strength</t>
   </si>
   <si>
@@ -2384,7 +2408,7 @@
     <t>The enemy feels so hopeless and depressed. This is a Stat reduction prefix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
   </si>
   <si>
-    <t>Lifes Bloody Sigil</t>
+    <t>Life's Bloody Sigill</t>
   </si>
   <si>
     <t>Draw the sigil on the ground I the enemies blood and feel life flow into you. This is a life stealing enchantment. If you are a vampire these have a chance to fire twice based on your class bonus. If you are not a vampire, these will fire once - at the end of the enemy round assuming you or them are not dead. Vampires have a chance for this to fire as part of their attack and after their enemies attack. These only stack if you are a vampire, other wise its your best one.</t>
@@ -2405,7 +2429,7 @@
     <t>Loss of Will</t>
   </si>
   <si>
-    <t>The enemy just looses the will to live. This is a Stat reduction prefix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
+    <t>The enemy just looses the will to live. This is a Stat reduction suffix. This will reduce all enemy stats by a specific amount. You may only have one of these on your items, having multiple will not stack the bonus and we only take the first one we find, as opposed to attempting to figure out your best one.</t>
   </si>
   <si>
     <t>Purgatory's Lost Enchantment</t>
@@ -2444,7 +2468,7 @@
     <t>The enemy breaks their brain trying to escape your raging enchantments</t>
   </si>
   <si>
-    <t>Blood Curtling Prayer</t>
+    <t>Blood Curdling Prayer</t>
   </si>
   <si>
     <t>This prayer will make the enemies blood curdle.</t>
@@ -2555,7 +2579,7 @@
     <t>This relic is best suited for a Vampire as it increases their stats and class bonuses as well as gives other Vampire specific enhancements. This is known as a kill enchantment. That is the damage on it will kill in conjunction with the life stealing.</t>
   </si>
   <si>
-    <t>Dextrous Lies</t>
+    <t>Dexterous Lies</t>
   </si>
   <si>
     <t>The enemy shrieks in agony and falls to their knees.</t>
@@ -2567,7 +2591,7 @@
     <t>This enchantment is best suited for a Fighter as it increases their stats and class bonuses as well as gives other Fighter specific enhancements.</t>
   </si>
   <si>
-    <t>Heretics Maddness</t>
+    <t>Heretics Madness</t>
   </si>
   <si>
     <t>This enchantment is best suited for a Heretic as it increases their stats and class bonuses as well as gives other Heretic specific enhancements.</t>
@@ -2609,7 +2633,7 @@
     <t>The enemy cannot contain their fear as the horse of death appears from the fog that surrounds them.</t>
   </si>
   <si>
-    <t>Satans Delicious Flesh Ripper</t>
+    <t>Satan's Delicious Flesh Ripper</t>
   </si>
   <si>
     <t>The enemy screams as you rip the flesh from their bones and lay it upon the ground.</t>
@@ -2705,7 +2729,7 @@
     <t>Seal of Demonic Fury</t>
   </si>
   <si>
-    <t>Feel the rage of the demons corse through your viens child.</t>
+    <t>Feel the rage of the demons course through your veins child.</t>
   </si>
   <si>
     <t>Heretics Insanity of the Mind</t>
@@ -2735,7 +2759,7 @@
     <t>Deaths Shadowy Grip</t>
   </si>
   <si>
-    <t>As you pick up your hammer, you feel the spectre of death reach through out your soul and grip the hammer with immense strength.</t>
+    <t>As you pick up your hammer, you feel the specter of death reach through out your soul and grip the hammer with immense strength.</t>
   </si>
   <si>
     <t>Cosmic Interference</t>
@@ -2810,7 +2834,7 @@
     <t>This enchantment will make you able to take on even the strongest of foes, provided you don't mind returning to the shackles that once bound you.</t>
   </si>
   <si>
-    <t>Lifes Final Breath</t>
+    <t>Life's Final Breath</t>
   </si>
   <si>
     <t>Take a final breath child. Lash the damage out at the expense of all else.</t>
@@ -16706,7 +16730,7 @@
         <v>339</v>
       </c>
       <c r="C142" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="L142">
         <v>0</v>
@@ -16792,10 +16816,10 @@
         <v>337</v>
       </c>
       <c r="B143" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C143" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="I143">
         <v>0.1451</v>
@@ -16884,10 +16908,10 @@
         <v>169</v>
       </c>
       <c r="B144" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C144" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="N144">
         <v>0</v>
@@ -16976,10 +17000,10 @@
         <v>338</v>
       </c>
       <c r="B145" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C145" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H145">
         <v>0.1132</v>
@@ -17068,10 +17092,10 @@
         <v>170</v>
       </c>
       <c r="B146" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C146" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N146">
         <v>0</v>
@@ -17160,10 +17184,10 @@
         <v>168</v>
       </c>
       <c r="B147" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C147" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="I147">
         <v>0.1722</v>
@@ -17258,10 +17282,10 @@
         <v>171</v>
       </c>
       <c r="B148" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C148" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N148">
         <v>0</v>
@@ -17350,10 +17374,10 @@
         <v>172</v>
       </c>
       <c r="B149" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C149" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N149">
         <v>0</v>
@@ -17442,10 +17466,10 @@
         <v>173</v>
       </c>
       <c r="B150" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C150" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N150">
         <v>0</v>
@@ -17534,10 +17558,10 @@
         <v>255</v>
       </c>
       <c r="B151" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C151" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L151">
         <v>0</v>
@@ -17623,10 +17647,10 @@
         <v>174</v>
       </c>
       <c r="B152" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C152" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="N152">
         <v>0</v>
@@ -17715,10 +17739,10 @@
         <v>256</v>
       </c>
       <c r="B153" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C153" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="L153">
         <v>0</v>
@@ -17807,10 +17831,10 @@
         <v>175</v>
       </c>
       <c r="B154" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C154" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K154">
         <v>0.1718</v>
@@ -17905,10 +17929,10 @@
         <v>340</v>
       </c>
       <c r="B155" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C155" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D155">
         <v>0.0681</v>
@@ -18018,10 +18042,10 @@
         <v>176</v>
       </c>
       <c r="B156" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C156" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="J156">
         <v>0.1667</v>
@@ -18116,10 +18140,10 @@
         <v>177</v>
       </c>
       <c r="B157" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C157" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G157">
         <v>0.1671</v>
@@ -18214,10 +18238,10 @@
         <v>178</v>
       </c>
       <c r="B158" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C158" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I158">
         <v>0.2059</v>
@@ -18312,10 +18336,10 @@
         <v>403</v>
       </c>
       <c r="B159" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C159" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="L159">
         <v>0</v>
@@ -18401,10 +18425,10 @@
         <v>31</v>
       </c>
       <c r="B160" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C160" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G160">
         <v>0.16</v>
@@ -18487,10 +18511,10 @@
         <v>179</v>
       </c>
       <c r="B161" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C161" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H161">
         <v>0.1449</v>
@@ -18582,10 +18606,10 @@
         <v>1011</v>
       </c>
       <c r="B162" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C162" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D162">
         <v>0.0713</v>
@@ -18692,10 +18716,10 @@
         <v>32</v>
       </c>
       <c r="B163" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C163" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I163">
         <v>0.1857</v>
@@ -18781,10 +18805,10 @@
         <v>1070</v>
       </c>
       <c r="B164" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C164" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D164">
         <v>0.0745</v>
@@ -18891,10 +18915,10 @@
         <v>266</v>
       </c>
       <c r="B165" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C165" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="L165">
         <v>0</v>
@@ -18980,10 +19004,10 @@
         <v>33</v>
       </c>
       <c r="B166" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C166" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H166">
         <v>0.137</v>
@@ -19066,10 +19090,10 @@
         <v>107</v>
       </c>
       <c r="B167" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C167" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="N167">
         <v>0</v>
@@ -19158,10 +19182,10 @@
         <v>34</v>
       </c>
       <c r="B168" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C168" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K168">
         <v>0.1644</v>
@@ -19247,10 +19271,10 @@
         <v>108</v>
       </c>
       <c r="B169" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C169" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N169">
         <v>0</v>
@@ -19339,10 +19363,10 @@
         <v>109</v>
       </c>
       <c r="B170" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C170" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="N170">
         <v>0</v>
@@ -19431,10 +19455,10 @@
         <v>35</v>
       </c>
       <c r="B171" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C171" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="J171">
         <v>0.1593</v>
@@ -19520,10 +19544,10 @@
         <v>268</v>
       </c>
       <c r="B172" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C172" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L172">
         <v>0</v>
@@ -19609,7 +19633,7 @@
         <v>258</v>
       </c>
       <c r="B173" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C173" t="s">
         <v>218</v>
@@ -19698,10 +19722,10 @@
         <v>404</v>
       </c>
       <c r="B174" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C174" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L174">
         <v>0</v>
@@ -19787,10 +19811,10 @@
         <v>405</v>
       </c>
       <c r="B175" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C175" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L175">
         <v>0</v>
@@ -19876,10 +19900,10 @@
         <v>343</v>
       </c>
       <c r="B176" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C176" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="K176">
         <v>0.1865</v>
@@ -19968,7 +19992,7 @@
         <v>259</v>
       </c>
       <c r="B177" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C177" t="s">
         <v>104</v>
@@ -20057,10 +20081,10 @@
         <v>344</v>
       </c>
       <c r="B178" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C178" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="J178">
         <v>0.1816</v>
@@ -20149,10 +20173,10 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C179" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="K179">
         <v>0.2159</v>
@@ -20247,7 +20271,7 @@
         <v>260</v>
       </c>
       <c r="B180" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C180" t="s">
         <v>106</v>
@@ -20336,10 +20360,10 @@
         <v>182</v>
       </c>
       <c r="B181" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C181" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K181">
         <v>0.2012</v>
@@ -20434,7 +20458,7 @@
         <v>261</v>
       </c>
       <c r="B182" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C182" t="s">
         <v>115</v>
@@ -20526,10 +20550,10 @@
         <v>183</v>
       </c>
       <c r="B183" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C183" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G183">
         <v>0.2029</v>
@@ -20624,10 +20648,10 @@
         <v>184</v>
       </c>
       <c r="B184" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C184" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I184">
         <v>0.233</v>
@@ -20722,7 +20746,7 @@
         <v>262</v>
       </c>
       <c r="B185" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C185" t="s">
         <v>121</v>
@@ -20811,10 +20835,10 @@
         <v>186</v>
       </c>
       <c r="B186" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C186" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I186">
         <v>0.2397</v>
@@ -20909,7 +20933,7 @@
         <v>263</v>
       </c>
       <c r="B187" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C187" t="s">
         <v>125</v>
@@ -20998,10 +21022,10 @@
         <v>1012</v>
       </c>
       <c r="B188" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C188" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D188">
         <v>0.0842</v>
@@ -21108,10 +21132,10 @@
         <v>180</v>
       </c>
       <c r="B189" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C189" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I189">
         <v>0.1924</v>
@@ -21206,10 +21230,10 @@
         <v>1071</v>
       </c>
       <c r="B190" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C190" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D190">
         <v>0.081</v>
@@ -21316,10 +21340,10 @@
         <v>48</v>
       </c>
       <c r="B191" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C191" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H191">
         <v>0.1687</v>
@@ -21402,10 +21426,10 @@
         <v>111</v>
       </c>
       <c r="B192" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C192" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N192">
         <v>0</v>
@@ -21494,10 +21518,10 @@
         <v>265</v>
       </c>
       <c r="B193" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C193" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="L193">
         <v>0</v>
@@ -21583,10 +21607,10 @@
         <v>112</v>
       </c>
       <c r="B194" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C194" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N194">
         <v>0</v>
@@ -21675,10 +21699,10 @@
         <v>110</v>
       </c>
       <c r="B195" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C195" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="N195">
         <v>0</v>
@@ -21767,10 +21791,10 @@
         <v>113</v>
       </c>
       <c r="B196" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C196" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N196">
         <v>0</v>
@@ -21859,10 +21883,10 @@
         <v>114</v>
       </c>
       <c r="B197" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C197" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="N197">
         <v>0</v>
@@ -21951,10 +21975,10 @@
         <v>444</v>
       </c>
       <c r="B198" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C198" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L198">
         <v>0</v>
@@ -22049,10 +22073,10 @@
         <v>445</v>
       </c>
       <c r="B199" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C199" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="L199">
         <v>0</v>
@@ -22147,10 +22171,10 @@
         <v>187</v>
       </c>
       <c r="B200" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C200" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="N200">
         <v>0</v>
@@ -22239,10 +22263,10 @@
         <v>267</v>
       </c>
       <c r="B201" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C201" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="L201">
         <v>0</v>
@@ -22328,10 +22352,10 @@
         <v>188</v>
       </c>
       <c r="B202" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C202" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N202">
         <v>0</v>
@@ -22420,10 +22444,10 @@
         <v>45</v>
       </c>
       <c r="B203" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C203" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D203">
         <v>0.0777</v>
@@ -22533,10 +22557,10 @@
         <v>189</v>
       </c>
       <c r="B204" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C204" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N204">
         <v>0</v>
@@ -22625,10 +22649,10 @@
         <v>192</v>
       </c>
       <c r="B205" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C205" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="N205">
         <v>0</v>
@@ -22717,10 +22741,10 @@
         <v>269</v>
       </c>
       <c r="B206" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C206" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="L206">
         <v>0</v>
@@ -22806,10 +22830,10 @@
         <v>49</v>
       </c>
       <c r="B207" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C207" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="K207">
         <v>0.2306</v>
@@ -22895,10 +22919,10 @@
         <v>50</v>
       </c>
       <c r="B208" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C208" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="J208">
         <v>0.2115</v>
@@ -22984,10 +23008,10 @@
         <v>341</v>
       </c>
       <c r="B209" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C209" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G209">
         <v>0.1814</v>
@@ -23076,10 +23100,10 @@
         <v>346</v>
       </c>
       <c r="B210" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C210" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H210">
         <v>0.1846</v>
@@ -23168,10 +23192,10 @@
         <v>96</v>
       </c>
       <c r="B211" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C211" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="I211">
         <v>0.2735</v>
@@ -23266,10 +23290,10 @@
         <v>342</v>
       </c>
       <c r="B212" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C212" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="I212">
         <v>0.2195</v>
@@ -23358,10 +23382,10 @@
         <v>193</v>
       </c>
       <c r="B213" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C213" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="K213">
         <v>0.2379</v>
@@ -23456,10 +23480,10 @@
         <v>185</v>
       </c>
       <c r="B214" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C214" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H214">
         <v>0.1608</v>
@@ -23551,10 +23575,10 @@
         <v>194</v>
       </c>
       <c r="B215" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C215" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="J215">
         <v>0.2264</v>
@@ -23649,10 +23673,10 @@
         <v>197</v>
       </c>
       <c r="B216" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C216" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="I216">
         <v>0.2668</v>
@@ -23747,10 +23771,10 @@
         <v>190</v>
       </c>
       <c r="B217" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C217" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="N217">
         <v>0</v>
@@ -23839,10 +23863,10 @@
         <v>272</v>
       </c>
       <c r="B218" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C218" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L218">
         <v>0</v>
@@ -23928,10 +23952,10 @@
         <v>191</v>
       </c>
       <c r="B219" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C219" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N219">
         <v>0</v>
@@ -24020,10 +24044,10 @@
         <v>406</v>
       </c>
       <c r="B220" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C220" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="L220">
         <v>0</v>
@@ -24109,10 +24133,10 @@
         <v>407</v>
       </c>
       <c r="B221" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C221" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="L221">
         <v>0</v>
@@ -24201,10 +24225,10 @@
         <v>270</v>
       </c>
       <c r="B222" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C222" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="L222">
         <v>0</v>
@@ -24290,10 +24314,10 @@
         <v>1013</v>
       </c>
       <c r="B223" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C223" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D223">
         <v>0.0906</v>
@@ -24400,10 +24424,10 @@
         <v>1072</v>
       </c>
       <c r="B224" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C224" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D224">
         <v>0.0939</v>
@@ -24510,10 +24534,10 @@
         <v>198</v>
       </c>
       <c r="B225" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C225" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="N225">
         <v>0</v>
@@ -24602,10 +24626,10 @@
         <v>271</v>
       </c>
       <c r="B226" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C226" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L226">
         <v>0</v>
@@ -24691,10 +24715,10 @@
         <v>93</v>
       </c>
       <c r="B227" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C227" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D227">
         <v>0.0971</v>
@@ -24783,10 +24807,10 @@
         <v>345</v>
       </c>
       <c r="B228" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C228" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D228">
         <v>0.0874</v>
@@ -24896,10 +24920,10 @@
         <v>199</v>
       </c>
       <c r="B229" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C229" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="N229">
         <v>0</v>
@@ -24988,10 +25012,10 @@
         <v>46</v>
       </c>
       <c r="B230" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C230" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G230">
         <v>0.2171</v>
@@ -25083,10 +25107,10 @@
         <v>200</v>
       </c>
       <c r="B231" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C231" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="N231">
         <v>0</v>
@@ -25175,10 +25199,10 @@
         <v>201</v>
       </c>
       <c r="B232" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C232" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="N232">
         <v>0</v>
@@ -25267,10 +25291,10 @@
         <v>47</v>
       </c>
       <c r="B233" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C233" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="I233">
         <v>0.2532</v>
@@ -25356,10 +25380,10 @@
         <v>446</v>
       </c>
       <c r="B234" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C234" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="L234">
         <v>0</v>
@@ -25454,10 +25478,10 @@
         <v>60</v>
       </c>
       <c r="B235" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C235" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D235">
         <v>0.1003</v>
@@ -25567,10 +25591,10 @@
         <v>195</v>
       </c>
       <c r="B236" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C236" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="G236">
         <v>0.2314</v>
@@ -25665,10 +25689,10 @@
         <v>127</v>
       </c>
       <c r="B237" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C237" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="N237">
         <v>0</v>
@@ -25757,10 +25781,10 @@
         <v>128</v>
       </c>
       <c r="B238" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C238" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="N238">
         <v>0</v>
@@ -25849,10 +25873,10 @@
         <v>196</v>
       </c>
       <c r="B239" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C239" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="H239">
         <v>0.1925</v>
@@ -25944,10 +25968,10 @@
         <v>129</v>
       </c>
       <c r="B240" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C240" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="N240">
         <v>0</v>
@@ -26036,10 +26060,10 @@
         <v>350</v>
       </c>
       <c r="B241" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C241" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="L241">
         <v>0</v>
@@ -26134,10 +26158,10 @@
         <v>130</v>
       </c>
       <c r="B242" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C242" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="N242">
         <v>0</v>
@@ -26226,10 +26250,10 @@
         <v>131</v>
       </c>
       <c r="B243" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C243" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="N243">
         <v>0</v>
@@ -26318,10 +26342,10 @@
         <v>352</v>
       </c>
       <c r="B244" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C244" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="L244">
         <v>0</v>
@@ -26416,10 +26440,10 @@
         <v>132</v>
       </c>
       <c r="B245" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C245" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="N245">
         <v>0</v>
@@ -26508,10 +26532,10 @@
         <v>273</v>
       </c>
       <c r="B246" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C246" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="L246">
         <v>0</v>
@@ -26597,10 +26621,10 @@
         <v>274</v>
       </c>
       <c r="B247" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C247" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="L247">
         <v>0</v>
@@ -26686,10 +26710,10 @@
         <v>202</v>
       </c>
       <c r="B248" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C248" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="N248">
         <v>0</v>
@@ -26778,10 +26802,10 @@
         <v>347</v>
       </c>
       <c r="B249" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C249" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="L249">
         <v>0</v>
@@ -26876,10 +26900,10 @@
         <v>348</v>
       </c>
       <c r="B250" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C250" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="L250">
         <v>0</v>
@@ -26974,10 +26998,10 @@
         <v>349</v>
       </c>
       <c r="B251" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C251" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="L251">
         <v>0</v>
@@ -27072,10 +27096,10 @@
         <v>275</v>
       </c>
       <c r="B252" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C252" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="L252">
         <v>0</v>
@@ -27161,10 +27185,10 @@
         <v>351</v>
       </c>
       <c r="B253" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C253" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="L253">
         <v>0</v>
@@ -27259,10 +27283,10 @@
         <v>277</v>
       </c>
       <c r="B254" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C254" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="L254">
         <v>0</v>
@@ -27348,10 +27372,10 @@
         <v>1014</v>
       </c>
       <c r="B255" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C255" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D255">
         <v>0.1068</v>
@@ -27458,10 +27482,10 @@
         <v>408</v>
       </c>
       <c r="B256" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C256" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="L256">
         <v>0</v>
@@ -27547,10 +27571,10 @@
         <v>1073</v>
       </c>
       <c r="B257" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C257" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D257">
         <v>0.1035</v>
@@ -27657,10 +27681,10 @@
         <v>276</v>
       </c>
       <c r="B258" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C258" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="L258">
         <v>0</v>
@@ -27749,10 +27773,10 @@
         <v>282</v>
       </c>
       <c r="B259" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C259" t="s">
-        <v>121</v>
+        <v>568</v>
       </c>
       <c r="L259">
         <v>0</v>
@@ -27838,10 +27862,10 @@
         <v>409</v>
       </c>
       <c r="B260" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C260" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="L260">
         <v>0</v>
@@ -27927,10 +27951,10 @@
         <v>283</v>
       </c>
       <c r="B261" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C261" t="s">
-        <v>125</v>
+        <v>572</v>
       </c>
       <c r="L261">
         <v>0</v>
@@ -28016,10 +28040,10 @@
         <v>65</v>
       </c>
       <c r="B262" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="C262" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="J262">
         <v>0.2488</v>
@@ -28105,10 +28129,10 @@
         <v>284</v>
       </c>
       <c r="B263" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="C263" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="L263">
         <v>0</v>
@@ -28194,10 +28218,10 @@
         <v>353</v>
       </c>
       <c r="B264" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="C264" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="L264">
         <v>0</v>
@@ -28292,10 +28316,10 @@
         <v>61</v>
       </c>
       <c r="B265" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="C265" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="G265">
         <v>0.26</v>
@@ -28378,10 +28402,10 @@
         <v>354</v>
       </c>
       <c r="B266" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C266" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="L266">
         <v>0</v>
@@ -28476,10 +28500,10 @@
         <v>355</v>
       </c>
       <c r="B267" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="C267" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="L267">
         <v>0</v>
@@ -28574,10 +28598,10 @@
         <v>62</v>
       </c>
       <c r="B268" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="C268" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="I268">
         <v>0.287</v>
@@ -28663,10 +28687,10 @@
         <v>356</v>
       </c>
       <c r="B269" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="C269" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="L269">
         <v>0</v>
@@ -28761,10 +28785,10 @@
         <v>63</v>
       </c>
       <c r="B270" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C270" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="H270">
         <v>0.2084</v>
@@ -28847,10 +28871,10 @@
         <v>357</v>
       </c>
       <c r="B271" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="C271" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="L271">
         <v>0</v>
@@ -28945,10 +28969,10 @@
         <v>1015</v>
       </c>
       <c r="B272" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="C272" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="D272">
         <v>0.1132</v>
@@ -29055,10 +29079,10 @@
         <v>64</v>
       </c>
       <c r="B273" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C273" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="K273">
         <v>0.2747</v>
@@ -29144,10 +29168,10 @@
         <v>1074</v>
       </c>
       <c r="B274" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C274" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="D274">
         <v>0.11</v>
@@ -29254,10 +29278,10 @@
         <v>203</v>
       </c>
       <c r="B275" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="C275" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="N275">
         <v>0</v>
@@ -29346,10 +29370,10 @@
         <v>204</v>
       </c>
       <c r="B276" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C276" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="N276">
         <v>0</v>
@@ -29438,7 +29462,7 @@
         <v>278</v>
       </c>
       <c r="B277" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="C277" t="s">
         <v>218</v>
@@ -29527,10 +29551,10 @@
         <v>205</v>
       </c>
       <c r="B278" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C278" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="N278">
         <v>0</v>
@@ -29619,7 +29643,7 @@
         <v>279</v>
       </c>
       <c r="B279" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="C279" t="s">
         <v>104</v>
@@ -29708,10 +29732,10 @@
         <v>206</v>
       </c>
       <c r="B280" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="C280" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="N280">
         <v>0</v>
@@ -29800,7 +29824,7 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="C281" t="s">
         <v>106</v>
@@ -29889,10 +29913,10 @@
         <v>208</v>
       </c>
       <c r="B282" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="C282" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="N282">
         <v>0</v>
@@ -29981,10 +30005,10 @@
         <v>94</v>
       </c>
       <c r="B283" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="C283" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="D283">
         <v>0.1165</v>
@@ -30073,7 +30097,7 @@
         <v>281</v>
       </c>
       <c r="B284" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C284" t="s">
         <v>115</v>
@@ -30165,10 +30189,10 @@
         <v>286</v>
       </c>
       <c r="B285" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C285" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="L285">
         <v>0</v>
@@ -30254,10 +30278,10 @@
         <v>207</v>
       </c>
       <c r="B286" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="C286" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="N286">
         <v>0</v>
@@ -30346,10 +30370,10 @@
         <v>410</v>
       </c>
       <c r="B287" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="C287" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="L287">
         <v>0</v>
@@ -30435,10 +30459,10 @@
         <v>411</v>
       </c>
       <c r="B288" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="C288" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="L288">
         <v>0</v>
@@ -30524,10 +30548,10 @@
         <v>209</v>
       </c>
       <c r="B289" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C289" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="N289">
         <v>0</v>
@@ -30616,10 +30640,10 @@
         <v>75</v>
       </c>
       <c r="B290" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="C290" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="D290">
         <v>0.1261</v>
@@ -30729,10 +30753,10 @@
         <v>287</v>
       </c>
       <c r="B291" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C291" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="L291">
         <v>0</v>
@@ -30818,10 +30842,10 @@
         <v>285</v>
       </c>
       <c r="B292" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="C292" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="L292">
         <v>0</v>
@@ -30907,10 +30931,10 @@
         <v>358</v>
       </c>
       <c r="B293" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C293" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="L293">
         <v>0</v>
@@ -31005,10 +31029,10 @@
         <v>359</v>
       </c>
       <c r="B294" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C294" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="L294">
         <v>0</v>
@@ -31103,10 +31127,10 @@
         <v>361</v>
       </c>
       <c r="B295" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C295" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="L295">
         <v>0</v>
@@ -31201,10 +31225,10 @@
         <v>360</v>
       </c>
       <c r="B296" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="C296" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="L296">
         <v>0</v>
@@ -31299,10 +31323,10 @@
         <v>362</v>
       </c>
       <c r="B297" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C297" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="L297">
         <v>0</v>
@@ -31397,10 +31421,10 @@
         <v>1016</v>
       </c>
       <c r="B298" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="C298" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="D298">
         <v>0.1229</v>
@@ -31507,10 +31531,10 @@
         <v>363</v>
       </c>
       <c r="B299" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="C299" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="L299">
         <v>0</v>
@@ -31605,10 +31629,10 @@
         <v>1075</v>
       </c>
       <c r="B300" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="C300" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="D300">
         <v>0.1197</v>
@@ -31715,10 +31739,10 @@
         <v>288</v>
       </c>
       <c r="B301" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C301" t="s">
-        <v>218</v>
+        <v>647</v>
       </c>
       <c r="L301">
         <v>0</v>
@@ -31804,10 +31828,10 @@
         <v>210</v>
       </c>
       <c r="B302" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C302" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="N302">
         <v>0</v>
@@ -31896,10 +31920,10 @@
         <v>289</v>
       </c>
       <c r="B303" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="C303" t="s">
-        <v>104</v>
+        <v>651</v>
       </c>
       <c r="L303">
         <v>0</v>
@@ -31985,10 +32009,10 @@
         <v>290</v>
       </c>
       <c r="B304" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="C304" t="s">
-        <v>106</v>
+        <v>653</v>
       </c>
       <c r="L304">
         <v>0</v>
@@ -32074,10 +32098,10 @@
         <v>211</v>
       </c>
       <c r="B305" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="C305" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="N305">
         <v>0</v>
@@ -32166,10 +32190,10 @@
         <v>292</v>
       </c>
       <c r="B306" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="C306" t="s">
-        <v>121</v>
+        <v>568</v>
       </c>
       <c r="L306">
         <v>0</v>
@@ -32255,10 +32279,10 @@
         <v>212</v>
       </c>
       <c r="B307" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="C307" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="N307">
         <v>0</v>
@@ -32347,10 +32371,10 @@
         <v>295</v>
       </c>
       <c r="B308" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="C308" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="L308">
         <v>0</v>
@@ -32436,10 +32460,10 @@
         <v>296</v>
       </c>
       <c r="B309" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="C309" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="L309">
         <v>0</v>
@@ -32525,10 +32549,10 @@
         <v>214</v>
       </c>
       <c r="B310" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="C310" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="N310">
         <v>0</v>
@@ -32617,10 +32641,10 @@
         <v>213</v>
       </c>
       <c r="B311" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="C311" t="s">
-        <v>660</v>
+        <v>666</v>
       </c>
       <c r="N311">
         <v>0</v>
@@ -32709,10 +32733,10 @@
         <v>215</v>
       </c>
       <c r="B312" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="C312" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="N312">
         <v>0</v>
@@ -32801,10 +32825,10 @@
         <v>216</v>
       </c>
       <c r="B313" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="C313" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="N313">
         <v>0</v>
@@ -32893,10 +32917,10 @@
         <v>447</v>
       </c>
       <c r="B314" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="C314" t="s">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="L314">
         <v>0</v>
@@ -32991,10 +33015,10 @@
         <v>76</v>
       </c>
       <c r="B315" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="C315" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="G315">
         <v>0.2814</v>
@@ -33089,10 +33113,10 @@
         <v>217</v>
       </c>
       <c r="B316" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="C316" t="s">
-        <v>670</v>
+        <v>676</v>
       </c>
       <c r="N316">
         <v>0</v>
@@ -33181,10 +33205,10 @@
         <v>448</v>
       </c>
       <c r="B317" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="C317" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
       <c r="L317">
         <v>0</v>
@@ -33279,10 +33303,10 @@
         <v>297</v>
       </c>
       <c r="B318" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="C318" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="L318">
         <v>0</v>
@@ -33371,10 +33395,10 @@
         <v>77</v>
       </c>
       <c r="B319" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="C319" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="I319">
         <v>0.3005</v>
@@ -33460,10 +33484,10 @@
         <v>298</v>
       </c>
       <c r="B320" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="C320" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="L320">
         <v>0</v>
@@ -33549,10 +33573,10 @@
         <v>78</v>
       </c>
       <c r="B321" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="C321" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="H321">
         <v>0.2243</v>
@@ -33635,10 +33659,10 @@
         <v>364</v>
       </c>
       <c r="B322" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
       <c r="C322" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="L322">
         <v>0</v>
@@ -33733,10 +33757,10 @@
         <v>79</v>
       </c>
       <c r="B323" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="C323" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="K323">
         <v>0.2968</v>
@@ -33822,10 +33846,10 @@
         <v>365</v>
       </c>
       <c r="B324" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="C324" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="L324">
         <v>0</v>
@@ -33920,10 +33944,10 @@
         <v>367</v>
       </c>
       <c r="B325" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="C325" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c r="L325">
         <v>0</v>
@@ -34018,10 +34042,10 @@
         <v>368</v>
       </c>
       <c r="B326" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="C326" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="L326">
         <v>0</v>
@@ -34116,10 +34140,10 @@
         <v>80</v>
       </c>
       <c r="B327" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c r="C327" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c r="J327">
         <v>0.2787</v>
@@ -34205,10 +34229,10 @@
         <v>413</v>
       </c>
       <c r="B328" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="C328" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
       <c r="L328">
         <v>0</v>
@@ -34294,7 +34318,7 @@
         <v>293</v>
       </c>
       <c r="B329" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="C329" t="s">
         <v>125</v>
@@ -34383,10 +34407,10 @@
         <v>1017</v>
       </c>
       <c r="B330" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="C330" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="D330">
         <v>0.1326</v>
@@ -34493,10 +34517,10 @@
         <v>1076</v>
       </c>
       <c r="B331" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="C331" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="D331">
         <v>0.1294</v>
@@ -34603,7 +34627,7 @@
         <v>294</v>
       </c>
       <c r="B332" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
       <c r="C332" t="s">
         <v>131</v>
@@ -34692,10 +34716,10 @@
         <v>223</v>
       </c>
       <c r="B333" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="C333" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="N333">
         <v>0</v>
@@ -34784,10 +34808,10 @@
         <v>299</v>
       </c>
       <c r="B334" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="C334" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="L334">
         <v>0</v>
@@ -34873,10 +34897,10 @@
         <v>366</v>
       </c>
       <c r="B335" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
       <c r="C335" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="L335">
         <v>0</v>
@@ -34971,10 +34995,10 @@
         <v>300</v>
       </c>
       <c r="B336" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="C336" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="L336">
         <v>0</v>
@@ -35060,10 +35084,10 @@
         <v>301</v>
       </c>
       <c r="B337" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="C337" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L337">
         <v>0</v>
@@ -35149,10 +35173,10 @@
         <v>369</v>
       </c>
       <c r="B338" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="C338" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="L338">
         <v>0</v>
@@ -35247,10 +35271,10 @@
         <v>370</v>
       </c>
       <c r="B339" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="C339" t="s">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c r="L339">
         <v>0</v>
@@ -35345,10 +35369,10 @@
         <v>412</v>
       </c>
       <c r="B340" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="C340" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c r="L340">
         <v>0</v>
@@ -35434,10 +35458,10 @@
         <v>371</v>
       </c>
       <c r="B341" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="C341" t="s">
-        <v>718</v>
+        <v>724</v>
       </c>
       <c r="L341">
         <v>0</v>
@@ -35532,10 +35556,10 @@
         <v>373</v>
       </c>
       <c r="B342" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="C342" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
       <c r="L342">
         <v>0</v>
@@ -35630,10 +35654,10 @@
         <v>218</v>
       </c>
       <c r="B343" t="s">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="C343" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="N343">
         <v>0</v>
@@ -35722,10 +35746,10 @@
         <v>415</v>
       </c>
       <c r="B344" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="C344" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="L344">
         <v>0</v>
@@ -35811,10 +35835,10 @@
         <v>219</v>
       </c>
       <c r="B345" t="s">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="C345" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="N345">
         <v>0</v>
@@ -35903,10 +35927,10 @@
         <v>1018</v>
       </c>
       <c r="B346" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
       <c r="C346" t="s">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="D346">
         <v>0.139</v>
@@ -36013,10 +36037,10 @@
         <v>1077</v>
       </c>
       <c r="B347" t="s">
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="C347" t="s">
-        <v>730</v>
+        <v>736</v>
       </c>
       <c r="D347">
         <v>0.1358</v>
@@ -36126,10 +36150,10 @@
         <v>220</v>
       </c>
       <c r="B348" t="s">
-        <v>731</v>
+        <v>737</v>
       </c>
       <c r="C348" t="s">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="N348">
         <v>0</v>
@@ -36221,10 +36245,10 @@
         <v>304</v>
       </c>
       <c r="B349" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="C349" t="s">
-        <v>106</v>
+        <v>653</v>
       </c>
       <c r="L349">
         <v>0</v>
@@ -36310,10 +36334,10 @@
         <v>307</v>
       </c>
       <c r="B350" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="C350" t="s">
-        <v>125</v>
+        <v>572</v>
       </c>
       <c r="L350">
         <v>0</v>
@@ -36399,10 +36423,10 @@
         <v>221</v>
       </c>
       <c r="B351" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="C351" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="N351">
         <v>0</v>
@@ -36491,10 +36515,10 @@
         <v>308</v>
       </c>
       <c r="B352" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="C352" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="L352">
         <v>0</v>
@@ -36580,10 +36604,10 @@
         <v>222</v>
       </c>
       <c r="B353" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="C353" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="N353">
         <v>0</v>
@@ -36672,10 +36696,10 @@
         <v>309</v>
       </c>
       <c r="B354" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="C354" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="L354">
         <v>0</v>
@@ -36761,10 +36785,10 @@
         <v>310</v>
       </c>
       <c r="B355" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="C355" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="L355">
         <v>0</v>
@@ -36850,10 +36874,10 @@
         <v>372</v>
       </c>
       <c r="B356" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="C356" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="L356">
         <v>0</v>
@@ -36948,10 +36972,10 @@
         <v>376</v>
       </c>
       <c r="B357" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="C357" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="L357">
         <v>0</v>
@@ -37046,10 +37070,10 @@
         <v>377</v>
       </c>
       <c r="B358" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="C358" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="L358">
         <v>0</v>
@@ -37144,10 +37168,10 @@
         <v>374</v>
       </c>
       <c r="B359" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="C359" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="L359">
         <v>0</v>
@@ -37242,10 +37266,10 @@
         <v>1019</v>
       </c>
       <c r="B360" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="C360" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="D360">
         <v>0.1455</v>
@@ -37352,10 +37376,10 @@
         <v>375</v>
       </c>
       <c r="B361" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="C361" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="L361">
         <v>0</v>
@@ -37450,10 +37474,10 @@
         <v>1078</v>
       </c>
       <c r="B362" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="C362" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="D362">
         <v>0.1423</v>
@@ -37563,10 +37587,10 @@
         <v>311</v>
       </c>
       <c r="B363" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="C363" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="L363">
         <v>0</v>
@@ -37652,10 +37676,10 @@
         <v>315</v>
       </c>
       <c r="B364" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C364" t="s">
-        <v>106</v>
+        <v>653</v>
       </c>
       <c r="L364">
         <v>0</v>
@@ -37741,10 +37765,10 @@
         <v>414</v>
       </c>
       <c r="B365" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="C365" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
       <c r="L365">
         <v>0</v>
@@ -37830,7 +37854,7 @@
         <v>302</v>
       </c>
       <c r="B366" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="C366" t="s">
         <v>218</v>
@@ -37919,10 +37943,10 @@
         <v>316</v>
       </c>
       <c r="B367" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="C367" t="s">
-        <v>115</v>
+        <v>770</v>
       </c>
       <c r="J367">
         <v>0</v>
@@ -38011,10 +38035,10 @@
         <v>317</v>
       </c>
       <c r="B368" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c r="C368" t="s">
-        <v>121</v>
+        <v>568</v>
       </c>
       <c r="L368">
         <v>0</v>
@@ -38100,7 +38124,7 @@
         <v>303</v>
       </c>
       <c r="B369" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
       <c r="C369" t="s">
         <v>104</v>
@@ -38189,10 +38213,10 @@
         <v>318</v>
       </c>
       <c r="B370" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="C370" t="s">
-        <v>125</v>
+        <v>572</v>
       </c>
       <c r="L370">
         <v>0</v>
@@ -38278,10 +38302,10 @@
         <v>319</v>
       </c>
       <c r="B371" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
       <c r="C371" t="s">
-        <v>131</v>
+        <v>340</v>
       </c>
       <c r="L371">
         <v>0</v>
@@ -38367,7 +38391,7 @@
         <v>305</v>
       </c>
       <c r="B372" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="C372" t="s">
         <v>115</v>
@@ -38462,10 +38486,10 @@
         <v>382</v>
       </c>
       <c r="B373" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
       <c r="C373" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
       <c r="L373">
         <v>0</v>
@@ -38560,7 +38584,7 @@
         <v>306</v>
       </c>
       <c r="B374" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="C374" t="s">
         <v>121</v>
@@ -38649,10 +38673,10 @@
         <v>383</v>
       </c>
       <c r="B375" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
       <c r="C375" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="L375">
         <v>0</v>
@@ -38747,10 +38771,10 @@
         <v>387</v>
       </c>
       <c r="B376" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="C376" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="L376">
         <v>0</v>
@@ -38845,10 +38869,10 @@
         <v>1020</v>
       </c>
       <c r="B377" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c r="C377" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
       <c r="D377">
         <v>0.1487</v>
@@ -38958,10 +38982,10 @@
         <v>378</v>
       </c>
       <c r="B378" t="s">
-        <v>778</v>
+        <v>785</v>
       </c>
       <c r="C378" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="L378">
         <v>0</v>
@@ -39056,10 +39080,10 @@
         <v>1079</v>
       </c>
       <c r="B379" t="s">
-        <v>779</v>
+        <v>786</v>
       </c>
       <c r="C379" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
       <c r="D379">
         <v>0.1519</v>
@@ -39169,10 +39193,10 @@
         <v>320</v>
       </c>
       <c r="B380" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
       <c r="C380" t="s">
-        <v>741</v>
+        <v>789</v>
       </c>
       <c r="L380">
         <v>0</v>
@@ -39258,10 +39282,10 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="C381" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="L381">
         <v>0</v>
@@ -39356,10 +39380,10 @@
         <v>321</v>
       </c>
       <c r="B382" t="s">
-        <v>784</v>
+        <v>792</v>
       </c>
       <c r="C382" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="L382">
         <v>0</v>
@@ -39445,10 +39469,10 @@
         <v>380</v>
       </c>
       <c r="B383" t="s">
-        <v>785</v>
+        <v>793</v>
       </c>
       <c r="C383" t="s">
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="L383">
         <v>0</v>
@@ -39543,10 +39567,10 @@
         <v>323</v>
       </c>
       <c r="B384" t="s">
-        <v>787</v>
+        <v>795</v>
       </c>
       <c r="C384" t="s">
-        <v>788</v>
+        <v>796</v>
       </c>
       <c r="L384">
         <v>0</v>
@@ -39638,10 +39662,10 @@
         <v>389</v>
       </c>
       <c r="B385" t="s">
-        <v>789</v>
+        <v>797</v>
       </c>
       <c r="C385" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="L385">
         <v>0</v>
@@ -39733,10 +39757,10 @@
         <v>381</v>
       </c>
       <c r="B386" t="s">
-        <v>791</v>
+        <v>799</v>
       </c>
       <c r="C386" t="s">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="L386">
         <v>0</v>
@@ -39831,10 +39855,10 @@
         <v>390</v>
       </c>
       <c r="B387" t="s">
-        <v>793</v>
+        <v>801</v>
       </c>
       <c r="C387" t="s">
-        <v>794</v>
+        <v>802</v>
       </c>
       <c r="D387">
         <v>0.1552</v>
@@ -39935,10 +39959,10 @@
         <v>312</v>
       </c>
       <c r="B388" t="s">
-        <v>795</v>
+        <v>803</v>
       </c>
       <c r="C388" t="s">
-        <v>796</v>
+        <v>804</v>
       </c>
       <c r="L388">
         <v>0</v>
@@ -40024,10 +40048,10 @@
         <v>1021</v>
       </c>
       <c r="B389" t="s">
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="C389" t="s">
-        <v>798</v>
+        <v>806</v>
       </c>
       <c r="D389">
         <v>0.1648</v>
@@ -40137,10 +40161,10 @@
         <v>1080</v>
       </c>
       <c r="B390" t="s">
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="C390" t="s">
-        <v>800</v>
+        <v>808</v>
       </c>
       <c r="D390">
         <v>0.1584</v>
@@ -40253,7 +40277,7 @@
         <v>313</v>
       </c>
       <c r="B391" t="s">
-        <v>801</v>
+        <v>809</v>
       </c>
       <c r="C391" t="s">
         <v>218</v>
@@ -40342,10 +40366,10 @@
         <v>393</v>
       </c>
       <c r="B392" t="s">
-        <v>802</v>
+        <v>810</v>
       </c>
       <c r="C392" t="s">
-        <v>803</v>
+        <v>811</v>
       </c>
       <c r="D392">
         <v>0.1681</v>
@@ -40449,10 +40473,10 @@
         <v>395</v>
       </c>
       <c r="B393" t="s">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="C393" t="s">
-        <v>805</v>
+        <v>813</v>
       </c>
       <c r="L393">
         <v>0</v>
@@ -40544,7 +40568,7 @@
         <v>314</v>
       </c>
       <c r="B394" t="s">
-        <v>806</v>
+        <v>814</v>
       </c>
       <c r="C394" t="s">
         <v>104</v>
@@ -40633,10 +40657,10 @@
         <v>417</v>
       </c>
       <c r="B395" t="s">
-        <v>807</v>
+        <v>815</v>
       </c>
       <c r="C395" t="s">
-        <v>808</v>
+        <v>816</v>
       </c>
       <c r="K395">
         <v>0.3556</v>
@@ -40731,10 +40755,10 @@
         <v>384</v>
       </c>
       <c r="B396" t="s">
-        <v>809</v>
+        <v>817</v>
       </c>
       <c r="C396" t="s">
-        <v>810</v>
+        <v>818</v>
       </c>
       <c r="L396">
         <v>0</v>
@@ -40832,10 +40856,10 @@
         <v>418</v>
       </c>
       <c r="B397" t="s">
-        <v>811</v>
+        <v>819</v>
       </c>
       <c r="C397" t="s">
-        <v>812</v>
+        <v>820</v>
       </c>
       <c r="H397">
         <v>0.256</v>
@@ -40933,10 +40957,10 @@
         <v>419</v>
       </c>
       <c r="B398" t="s">
-        <v>813</v>
+        <v>821</v>
       </c>
       <c r="C398" t="s">
-        <v>814</v>
+        <v>822</v>
       </c>
       <c r="J398">
         <v>0.3309</v>
@@ -41031,10 +41055,10 @@
         <v>385</v>
       </c>
       <c r="B399" t="s">
-        <v>815</v>
+        <v>823</v>
       </c>
       <c r="C399" t="s">
-        <v>816</v>
+        <v>824</v>
       </c>
       <c r="L399">
         <v>0</v>
@@ -41129,10 +41153,10 @@
         <v>1022</v>
       </c>
       <c r="B400" t="s">
-        <v>817</v>
+        <v>825</v>
       </c>
       <c r="C400" t="s">
-        <v>818</v>
+        <v>826</v>
       </c>
       <c r="D400">
         <v>0.1713</v>
@@ -41233,10 +41257,10 @@
         <v>420</v>
       </c>
       <c r="B401" t="s">
-        <v>819</v>
+        <v>827</v>
       </c>
       <c r="C401" t="s">
-        <v>820</v>
+        <v>828</v>
       </c>
       <c r="D401">
         <v>0.1745</v>
@@ -41337,10 +41361,10 @@
         <v>386</v>
       </c>
       <c r="B402" t="s">
-        <v>821</v>
+        <v>829</v>
       </c>
       <c r="C402" t="s">
-        <v>822</v>
+        <v>830</v>
       </c>
       <c r="L402">
         <v>0</v>
@@ -41435,10 +41459,10 @@
         <v>421</v>
       </c>
       <c r="B403" t="s">
-        <v>823</v>
+        <v>831</v>
       </c>
       <c r="C403" t="s">
-        <v>824</v>
+        <v>832</v>
       </c>
       <c r="L403">
         <v>0</v>
@@ -41527,10 +41551,10 @@
         <v>291</v>
       </c>
       <c r="B404" t="s">
-        <v>825</v>
+        <v>833</v>
       </c>
       <c r="C404" t="s">
-        <v>826</v>
+        <v>834</v>
       </c>
       <c r="D404">
         <v>0.1777</v>
@@ -41628,10 +41652,10 @@
         <v>322</v>
       </c>
       <c r="B405" t="s">
-        <v>827</v>
+        <v>835</v>
       </c>
       <c r="C405" t="s">
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="L405">
         <v>0</v>
@@ -41720,10 +41744,10 @@
         <v>422</v>
       </c>
       <c r="B406" t="s">
-        <v>829</v>
+        <v>837</v>
       </c>
       <c r="C406" t="s">
-        <v>830</v>
+        <v>838</v>
       </c>
       <c r="D406">
         <v>0.181</v>
@@ -41827,10 +41851,10 @@
         <v>388</v>
       </c>
       <c r="B407" t="s">
-        <v>831</v>
+        <v>839</v>
       </c>
       <c r="C407" t="s">
-        <v>832</v>
+        <v>840</v>
       </c>
       <c r="L407">
         <v>0</v>
@@ -41925,10 +41949,10 @@
         <v>423</v>
       </c>
       <c r="B408" t="s">
-        <v>833</v>
+        <v>841</v>
       </c>
       <c r="C408" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
       <c r="D408">
         <v>0.1842</v>
@@ -42026,10 +42050,10 @@
         <v>424</v>
       </c>
       <c r="B409" t="s">
-        <v>835</v>
+        <v>843</v>
       </c>
       <c r="C409" t="s">
-        <v>826</v>
+        <v>834</v>
       </c>
       <c r="E409">
         <v>0.13</v>
@@ -42124,10 +42148,10 @@
         <v>391</v>
       </c>
       <c r="B410" t="s">
-        <v>836</v>
+        <v>844</v>
       </c>
       <c r="C410" t="s">
-        <v>837</v>
+        <v>845</v>
       </c>
       <c r="G410">
         <v>0.3171</v>
@@ -42234,10 +42258,10 @@
         <v>425</v>
       </c>
       <c r="B411" t="s">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c r="C411" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
       <c r="D411">
         <v>0.1874</v>
@@ -42335,10 +42359,10 @@
         <v>392</v>
       </c>
       <c r="B412" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="C412" t="s">
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="D412">
         <v>0.1616</v>
@@ -42439,10 +42463,10 @@
         <v>426</v>
       </c>
       <c r="B413" t="s">
-        <v>842</v>
+        <v>850</v>
       </c>
       <c r="C413" t="s">
-        <v>843</v>
+        <v>851</v>
       </c>
       <c r="D413">
         <v>0.1906</v>
@@ -42546,10 +42570,10 @@
         <v>427</v>
       </c>
       <c r="B414" t="s">
-        <v>844</v>
+        <v>852</v>
       </c>
       <c r="C414" t="s">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="D414">
         <v>0.1939</v>
@@ -42650,10 +42674,10 @@
         <v>394</v>
       </c>
       <c r="B415" t="s">
-        <v>846</v>
+        <v>854</v>
       </c>
       <c r="C415" t="s">
-        <v>847</v>
+        <v>855</v>
       </c>
       <c r="D415">
         <v>0</v>
@@ -42760,10 +42784,10 @@
         <v>428</v>
       </c>
       <c r="B416" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
       <c r="C416" t="s">
-        <v>849</v>
+        <v>857</v>
       </c>
       <c r="D416">
         <v>0.2003</v>
@@ -42867,10 +42891,10 @@
         <v>429</v>
       </c>
       <c r="B417" t="s">
-        <v>850</v>
+        <v>858</v>
       </c>
       <c r="C417" t="s">
-        <v>851</v>
+        <v>859</v>
       </c>
       <c r="D417">
         <v>0.21</v>
@@ -42965,10 +42989,10 @@
         <v>416</v>
       </c>
       <c r="B418" t="s">
-        <v>852</v>
+        <v>860</v>
       </c>
       <c r="C418" t="s">
-        <v>853</v>
+        <v>861</v>
       </c>
       <c r="L418">
         <v>0</v>
@@ -43060,10 +43084,10 @@
         <v>430</v>
       </c>
       <c r="B419" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="C419" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E419">
         <v>0.15</v>
@@ -43158,10 +43182,10 @@
         <v>431</v>
       </c>
       <c r="B420" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="C420" t="s">
-        <v>851</v>
+        <v>859</v>
       </c>
       <c r="D420">
         <v>0.2068</v>
@@ -43256,10 +43280,10 @@
         <v>449</v>
       </c>
       <c r="B421" t="s">
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="C421" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E421">
         <v>0.17</v>
@@ -43360,10 +43384,10 @@
         <v>432</v>
       </c>
       <c r="B422" t="s">
-        <v>858</v>
+        <v>866</v>
       </c>
       <c r="C422" t="s">
-        <v>859</v>
+        <v>867</v>
       </c>
       <c r="D422">
         <v>0.2035</v>
@@ -43467,10 +43491,10 @@
         <v>433</v>
       </c>
       <c r="B423" t="s">
-        <v>860</v>
+        <v>868</v>
       </c>
       <c r="C423" t="s">
-        <v>861</v>
+        <v>869</v>
       </c>
       <c r="D423">
         <v>0.1971</v>
@@ -43574,10 +43598,10 @@
         <v>435</v>
       </c>
       <c r="B424" t="s">
-        <v>862</v>
+        <v>870</v>
       </c>
       <c r="C424" t="s">
-        <v>863</v>
+        <v>871</v>
       </c>
       <c r="G424">
         <v>0.3671</v>
@@ -43684,10 +43708,10 @@
         <v>434</v>
       </c>
       <c r="B425" t="s">
-        <v>864</v>
+        <v>872</v>
       </c>
       <c r="C425" t="s">
-        <v>865</v>
+        <v>873</v>
       </c>
       <c r="D425">
         <v>0.2132</v>
@@ -43803,10 +43827,10 @@
         <v>436</v>
       </c>
       <c r="B426" t="s">
-        <v>866</v>
+        <v>874</v>
       </c>
       <c r="C426" t="s">
-        <v>867</v>
+        <v>875</v>
       </c>
       <c r="G426">
         <v>0.3743</v>
@@ -43907,10 +43931,10 @@
         <v>1023</v>
       </c>
       <c r="B427" t="s">
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="C427" t="s">
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="D427">
         <v>0.2197</v>
@@ -44011,10 +44035,10 @@
         <v>437</v>
       </c>
       <c r="B428" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="C428" t="s">
-        <v>871</v>
+        <v>879</v>
       </c>
       <c r="D428">
         <v>0.2165</v>
@@ -44121,10 +44145,10 @@
         <v>438</v>
       </c>
       <c r="B429" t="s">
-        <v>872</v>
+        <v>880</v>
       </c>
       <c r="C429" t="s">
-        <v>873</v>
+        <v>881</v>
       </c>
       <c r="D429">
         <v>0.2229</v>
@@ -44237,10 +44261,10 @@
         <v>440</v>
       </c>
       <c r="B430" t="s">
-        <v>874</v>
+        <v>882</v>
       </c>
       <c r="C430" t="s">
-        <v>875</v>
+        <v>883</v>
       </c>
       <c r="G430">
         <v>0.3957</v>
@@ -44347,10 +44371,10 @@
         <v>439</v>
       </c>
       <c r="B431" t="s">
-        <v>876</v>
+        <v>884</v>
       </c>
       <c r="C431" t="s">
-        <v>877</v>
+        <v>885</v>
       </c>
       <c r="D431">
         <v>0</v>
@@ -44457,10 +44481,10 @@
         <v>452</v>
       </c>
       <c r="B432" t="s">
-        <v>878</v>
+        <v>886</v>
       </c>
       <c r="C432" t="s">
-        <v>879</v>
+        <v>887</v>
       </c>
       <c r="D432">
         <v>0.2261</v>
@@ -44576,10 +44600,10 @@
         <v>450</v>
       </c>
       <c r="B433" t="s">
-        <v>880</v>
+        <v>888</v>
       </c>
       <c r="C433" t="s">
-        <v>881</v>
+        <v>889</v>
       </c>
       <c r="H433">
         <v>0.3433</v>
@@ -44677,10 +44701,10 @@
         <v>455</v>
       </c>
       <c r="B434" t="s">
-        <v>882</v>
+        <v>890</v>
       </c>
       <c r="C434" t="s">
-        <v>883</v>
+        <v>891</v>
       </c>
       <c r="E434">
         <v>0.21</v>
@@ -44787,10 +44811,10 @@
         <v>456</v>
       </c>
       <c r="B435" t="s">
-        <v>884</v>
+        <v>892</v>
       </c>
       <c r="C435" t="s">
-        <v>885</v>
+        <v>893</v>
       </c>
       <c r="D435">
         <v>0.2326</v>
@@ -44906,10 +44930,10 @@
         <v>451</v>
       </c>
       <c r="B436" t="s">
-        <v>886</v>
+        <v>894</v>
       </c>
       <c r="C436" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="L436">
         <v>0</v>
@@ -45001,10 +45025,10 @@
         <v>457</v>
       </c>
       <c r="B437" t="s">
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="C437" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="D437">
         <v>0.2358</v>
@@ -45102,10 +45126,10 @@
         <v>458</v>
       </c>
       <c r="B438" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="C438" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="D438">
         <v>0.239</v>
@@ -45215,10 +45239,10 @@
         <v>453</v>
       </c>
       <c r="B439" t="s">
-        <v>892</v>
+        <v>900</v>
       </c>
       <c r="C439" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="G439">
         <v>0.41</v>
@@ -45322,10 +45346,10 @@
         <v>459</v>
       </c>
       <c r="B440" t="s">
-        <v>894</v>
+        <v>902</v>
       </c>
       <c r="C440" t="s">
-        <v>849</v>
+        <v>857</v>
       </c>
       <c r="D440">
         <v>0.2584</v>
@@ -45429,10 +45453,10 @@
         <v>454</v>
       </c>
       <c r="B441" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="C441" t="s">
-        <v>896</v>
+        <v>904</v>
       </c>
       <c r="D441">
         <v>0.2294</v>
@@ -45542,10 +45566,10 @@
         <v>460</v>
       </c>
       <c r="B442" t="s">
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="C442" t="s">
-        <v>851</v>
+        <v>859</v>
       </c>
       <c r="D442">
         <v>0.2423</v>
@@ -45640,10 +45664,10 @@
         <v>462</v>
       </c>
       <c r="B443" t="s">
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="C443" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="D443">
         <v>0.2455</v>
@@ -45744,10 +45768,10 @@
         <v>463</v>
       </c>
       <c r="B444" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="C444" t="s">
-        <v>859</v>
+        <v>867</v>
       </c>
       <c r="D444">
         <v>0.2519</v>
@@ -45848,10 +45872,10 @@
         <v>461</v>
       </c>
       <c r="B445" t="s">
-        <v>901</v>
+        <v>909</v>
       </c>
       <c r="C445" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E445">
         <v>0.23</v>
@@ -45949,10 +45973,10 @@
         <v>464</v>
       </c>
       <c r="B446" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="C446" t="s">
-        <v>861</v>
+        <v>869</v>
       </c>
       <c r="D446">
         <v>0.2552</v>
@@ -46050,10 +46074,10 @@
         <v>465</v>
       </c>
       <c r="B447" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="C447" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="G447">
         <v>0.4529</v>
@@ -46157,10 +46181,10 @@
         <v>1024</v>
       </c>
       <c r="B448" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="C448" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="D448">
         <v>0.2487</v>
@@ -46264,10 +46288,10 @@
         <v>466</v>
       </c>
       <c r="B449" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="C449" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="D449">
         <v>0.2616</v>
@@ -46380,10 +46404,10 @@
         <v>467</v>
       </c>
       <c r="B450" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="C450" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="L450">
         <v>0</v>
@@ -46472,10 +46496,10 @@
         <v>468</v>
       </c>
       <c r="B451" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="C451" t="s">
-        <v>912</v>
+        <v>920</v>
       </c>
       <c r="D451">
         <v>0.2681</v>
@@ -46585,10 +46609,10 @@
         <v>469</v>
       </c>
       <c r="B452" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
       <c r="C452" t="s">
-        <v>914</v>
+        <v>922</v>
       </c>
       <c r="D452">
         <v>0.2713</v>
@@ -46695,10 +46719,10 @@
         <v>474</v>
       </c>
       <c r="B453" t="s">
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="C453" t="s">
-        <v>916</v>
+        <v>924</v>
       </c>
       <c r="D453">
         <v>0.2874</v>
@@ -46802,10 +46826,10 @@
         <v>470</v>
       </c>
       <c r="B454" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
       <c r="C454" t="s">
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="D454">
         <v>0.281</v>
@@ -46915,10 +46939,10 @@
         <v>471</v>
       </c>
       <c r="B455" t="s">
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="C455" t="s">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="D455">
         <v>0.2648</v>
@@ -47022,10 +47046,10 @@
         <v>475</v>
       </c>
       <c r="B456" t="s">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="C456" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
       <c r="D456">
         <v>0.2906</v>
@@ -47144,10 +47168,10 @@
         <v>472</v>
       </c>
       <c r="B457" t="s">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="C457" t="s">
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="D457">
         <v>0.2777</v>
@@ -47254,10 +47278,10 @@
         <v>477</v>
       </c>
       <c r="B458" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="C458" t="s">
-        <v>926</v>
+        <v>934</v>
       </c>
       <c r="D458">
         <v>0.2971</v>
@@ -47376,10 +47400,10 @@
         <v>473</v>
       </c>
       <c r="B459" t="s">
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="C459" t="s">
-        <v>928</v>
+        <v>936</v>
       </c>
       <c r="D459">
         <v>0.2745</v>
@@ -47483,10 +47507,10 @@
         <v>1025</v>
       </c>
       <c r="B460" t="s">
-        <v>929</v>
+        <v>937</v>
       </c>
       <c r="C460" t="s">
-        <v>930</v>
+        <v>938</v>
       </c>
       <c r="D460">
         <v>0.2842</v>
@@ -47590,10 +47614,10 @@
         <v>478</v>
       </c>
       <c r="B461" t="s">
-        <v>931</v>
+        <v>939</v>
       </c>
       <c r="C461" t="s">
-        <v>932</v>
+        <v>940</v>
       </c>
       <c r="D461">
         <v>0.3</v>
@@ -47688,10 +47712,10 @@
         <v>476</v>
       </c>
       <c r="B462" t="s">
-        <v>933</v>
+        <v>941</v>
       </c>
       <c r="C462" t="s">
-        <v>934</v>
+        <v>942</v>
       </c>
       <c r="D462">
         <v>0.2939</v>
@@ -47807,10 +47831,10 @@
         <v>479</v>
       </c>
       <c r="B463" t="s">
-        <v>935</v>
+        <v>943</v>
       </c>
       <c r="C463" t="s">
-        <v>936</v>
+        <v>944</v>
       </c>
       <c r="D463">
         <v>0.3</v>
@@ -47926,10 +47950,10 @@
         <v>1026</v>
       </c>
       <c r="B464" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="C464" t="s">
-        <v>938</v>
+        <v>946</v>
       </c>
       <c r="D464">
         <v>0.3</v>

</xml_diff>